<commit_message>
Adiciona analise de técnicas
</commit_message>
<xml_diff>
--- a/copilot_x_especialista.xlsx
+++ b/copilot_x_especialista.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
   <si>
     <t>Técnica de rafatoração</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Refatoração copilot</t>
   </si>
   <si>
-    <t>Refatoração manual</t>
+    <t>Refatoração Guru</t>
   </si>
   <si>
     <t>Pull Up Constructor Body</t>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Consolidate Conditional Expression</t>
+  </si>
+  <si>
+    <t>Diferente s referencia</t>
   </si>
   <si>
     <t>Replace Magic Number With Symbolic Constant</t>
@@ -144,6 +147,9 @@
   </si>
   <si>
     <t>Replace Exception With Test</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
   <si>
     <t>Replace Method With Method Object</t>
@@ -693,167 +699,227 @@
         <v>22</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="C14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="21.75">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="31.5">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>6</v>

</xml_diff>